<commit_message>
Interfaz implementada parcialmente con countdown
</commit_message>
<xml_diff>
--- a/Lista de Asistencia.xlsx
+++ b/Lista de Asistencia.xlsx
@@ -130,7 +130,7 @@
   <tableColumns count="3">
     <tableColumn id="1" name="Numero de Lista"/>
     <tableColumn id="2" name="Nombre"/>
-    <tableColumn id="3" name="2024-11-15 17:01:23"/>
+    <tableColumn id="3" name="2024-11-15 17:18:48"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
 </table>
@@ -446,7 +446,7 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>2024-11-15 17:01:23</t>
+          <t>2024-11-15 17:18:48</t>
         </is>
       </c>
     </row>
@@ -476,7 +476,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Falta</t>
+          <t>Puntual</t>
         </is>
       </c>
     </row>
@@ -506,7 +506,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Falta</t>
+          <t>Puntual</t>
         </is>
       </c>
     </row>
@@ -521,7 +521,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Falta</t>
+          <t>Puntual</t>
         </is>
       </c>
     </row>
@@ -536,7 +536,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Falta</t>
+          <t>Puntual</t>
         </is>
       </c>
     </row>
@@ -551,7 +551,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Retardo</t>
+          <t>Puntual</t>
         </is>
       </c>
     </row>
@@ -581,7 +581,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Falta</t>
+          <t>Puntual</t>
         </is>
       </c>
     </row>
@@ -611,7 +611,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Falta</t>
+          <t>Puntual</t>
         </is>
       </c>
     </row>

</xml_diff>